<commit_message>
updated test csv with ppt
</commit_message>
<xml_diff>
--- a/test/admin/batch-template.xlsx
+++ b/test/admin/batch-template.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Title</t>
   </si>
@@ -72,10 +72,22 @@
     <t>This is a test to see if I can modify excel docs</t>
   </si>
   <si>
-    <t>Elder Scfrolls Legends no on Ipad</t>
-  </si>
-  <si>
     <t>Hearthstone Tournament</t>
+  </si>
+  <si>
+    <t>nested\test.pptx</t>
+  </si>
+  <si>
+    <t>Van Jones</t>
+  </si>
+  <si>
+    <t>Testing for nested pptx</t>
+  </si>
+  <si>
+    <t>Elder Scrolls Legends now on Ipad</t>
+  </si>
+  <si>
+    <t>Now 10% more awesome</t>
   </si>
 </sst>
 </file>
@@ -393,16 +405,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" bestFit="1" customWidth="1"/>
   </cols>
@@ -452,7 +464,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -466,7 +478,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -476,6 +488,20 @@
       </c>
       <c r="D5" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test CSV files
</commit_message>
<xml_diff>
--- a/test/admin/batch-template.xlsx
+++ b/test/admin/batch-template.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Title</t>
   </si>
@@ -88,12 +88,63 @@
   </si>
   <si>
     <t>Now 10% more awesome</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Rights</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>ExpirationDate</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>Copyright &amp;copy; 2017</t>
+  </si>
+  <si>
+    <t>American Bar Association</t>
+  </si>
+  <si>
+    <t>Copyright &amp;copy; 2018</t>
+  </si>
+  <si>
+    <t>Copyright &amp;copy; 2019</t>
+  </si>
+  <si>
+    <t>Copyright &amp;copy; 2020</t>
+  </si>
+  <si>
+    <t>Copyright &amp;copy; 2021</t>
+  </si>
+  <si>
+    <t>Tags:ROBOTS</t>
+  </si>
+  <si>
+    <t>FOLLOW</t>
+  </si>
+  <si>
+    <t>Tags:publishing_entity</t>
+  </si>
+  <si>
+    <t>PT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy:mm:dd\ hh:mm"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,8 +174,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,103 +461,221 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="str">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
         <f>T("-Path")</f>
         <v>-Path</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="3">
+        <v>42874.135416666664</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="3">
+        <v>42875.763194444444</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="3">
+        <v>42874.135416666664</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="3">
+        <v>42875.135416608799</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="3">
+        <v>42876.135416608799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test files and write settings
</commit_message>
<xml_diff>
--- a/test/admin/batch-template.xlsx
+++ b/test/admin/batch-template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Title</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Path</t>
+  </si>
+  <si>
+    <t>testx.pdf</t>
   </si>
 </sst>
 </file>
@@ -464,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +589,7 @@
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
@@ -678,6 +681,11 @@
       </c>
       <c r="K6" s="3">
         <v>42876.135416608799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>